<commit_message>
Generated mapping files to base comments on
Also added a different way to create mapping in mapping notebook when only parts of a zib are mapped.
</commit_message>
<xml_diff>
--- a/maps/LaboratoryTestResult.xlsx
+++ b/maps/LaboratoryTestResult.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nictiznl-my.sharepoint.com/personal/wouter_zanen_nictiz_nl/Documents/Documenten/GitHub/eu-nl-compared/maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="11_C29984414FA903520E1D8106792E2021C840DED0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35D14EDB-D157-48C3-9221-4E502477EAFF}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="11_C29984414FA903520E1D8106792E2021C840DED0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8857B574-C22E-469B-BEEB-CF5FEC5FA1B3}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="912" windowWidth="20112" windowHeight="12276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -264,10 +264,10 @@
     <t>LaboratoryTestResult.RelatedResult::LaboratoryTestResult</t>
   </si>
   <si>
-    <t>PanelOrBattery</t>
-  </si>
-  <si>
     <t>LaboratoryTestResult.ResultStatus</t>
+  </si>
+  <si>
+    <t>LaboratoryTestResult.PanelOrBattery</t>
   </si>
 </sst>
 </file>
@@ -613,16 +613,16 @@
   <dimension ref="A1:R59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="69.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="1" max="1" width="69.44140625" customWidth="1"/>
+    <col min="2" max="2" width="69.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +678,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -686,250 +686,250 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -937,17 +937,17 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>69</v>
       </c>
@@ -955,7 +955,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -963,27 +963,27 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>76</v>
       </c>
@@ -994,18 +994,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3af30693-c405-4a5b-908a-bd1dc294f76b" xsi:nil="true"/>
-    <Inhoud xmlns="b19602bd-a67a-4df8-b412-b401dd608f7a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b19602bd-a67a-4df8-b412-b401dd608f7a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BAFAE49EF5FC2A44A9A24B379C77993A" ma:contentTypeVersion="18" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="4e3f09d53704208a567efd423a8e8ffb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b19602bd-a67a-4df8-b412-b401dd608f7a" xmlns:ns3="3af30693-c405-4a5b-908a-bd1dc294f76b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5e8dd9eed0ce6952e5fe39cbc0c50bd" ns2:_="" ns3:_="">
     <xsd:import namespace="b19602bd-a67a-4df8-b412-b401dd608f7a"/>
@@ -1262,6 +1250,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3af30693-c405-4a5b-908a-bd1dc294f76b" xsi:nil="true"/>
+    <Inhoud xmlns="b19602bd-a67a-4df8-b412-b401dd608f7a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b19602bd-a67a-4df8-b412-b401dd608f7a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1272,23 +1272,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{150E1455-19EB-4AC0-BA9D-EE9CBCC1FEFB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b19602bd-a67a-4df8-b412-b401dd608f7a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="3af30693-c405-4a5b-908a-bd1dc294f76b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{569FF7CE-CFE6-4FA6-80F1-6CFE45CA983A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1307,6 +1290,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{150E1455-19EB-4AC0-BA9D-EE9CBCC1FEFB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b19602bd-a67a-4df8-b412-b401dd608f7a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3af30693-c405-4a5b-908a-bd1dc294f76b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D0E272B-3645-4028-A960-0B8D0057D9EE}">
   <ds:schemaRefs>

</xml_diff>